<commit_message>
changes for testxase and checklist doc
</commit_message>
<xml_diff>
--- a/TestCases_Checklist.xlsx
+++ b/TestCases_Checklist.xlsx
@@ -14,62 +14,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="F18">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAr0mBpB4
-Vladislav Leshko    (2023-02-25 09:19:20)
-можно попробовать через шифт или ктрл выбрать несколько преподов</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="F16">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAr0mBpB0
-Vladislav Leshko    (2023-02-25 09:18:09)
-отличный степ с проверкой радиобаттона для одного значения. просто на будущее - можно ещё проверить, что по дефолту один радиобаттон всегда прожат</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="F14">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAr0mBpBw
-Vladislav Leshko    (2023-02-25 09:14:44)
-а буквенные значения?</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="F13">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAr0mBpBs
-Vladislav Leshko    (2023-02-25 09:14:12)
-1) в этом и последующем тестах - почему бы не вынести в прекодишены 0 степ?
-2) почему бы не добавить кейс на проверку невалидных значений - цифры, символы?</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A1">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAr0mBpBo
-Vladislav Leshko    (2023-02-25 09:09:58)
-интересно, по какому принципу ты выставляла приоритет тест-кейсам?</t>
-      </text>
-    </comment>
-  </commentList>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhO+7yEOD1AUXmsmCI2jyVIOwxIHA=="/>
-    </ext>
-  </extLst>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5688,8 +5632,7 @@
       <formula1>"Passed,Failed,Skipped"</formula1>
     </dataValidation>
   </dataValidations>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>